<commit_message>
Update from PC 280423 2100 Final Configuration files.
</commit_message>
<xml_diff>
--- a/events/Tel_Mond_2023/competition_files/חריגים.xlsx
+++ b/events/Tel_Mond_2023/competition_files/חריגים.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>מס' חבר/ת.ז.</t>
   </si>
@@ -37,19 +37,52 @@
     <t>חריגה</t>
   </si>
   <si>
+    <t>56528482</t>
+  </si>
+  <si>
+    <t>בר הלוי יורם</t>
+  </si>
+  <si>
+    <t>קצר</t>
+  </si>
+  <si>
+    <t>503147001</t>
+  </si>
+  <si>
+    <t>נרשם לתחרותי אבל ללא כרטיס אלקטרוני</t>
+  </si>
+  <si>
     <t>340302652</t>
   </si>
   <si>
     <t>ברונפלד איתן</t>
   </si>
   <si>
-    <t>קצר</t>
-  </si>
-  <si>
     <t>509500778</t>
   </si>
   <si>
-    <t>נרשם לתחרותי אבל ללא כרטיס אלקטרוני</t>
+    <t>52674090</t>
+  </si>
+  <si>
+    <t>גוטהילף צבי</t>
+  </si>
+  <si>
+    <t>בינוני</t>
+  </si>
+  <si>
+    <t>543295075</t>
+  </si>
+  <si>
+    <t>22512727</t>
+  </si>
+  <si>
+    <t>גורקה אורנה</t>
+  </si>
+  <si>
+    <t>קצרצר</t>
+  </si>
+  <si>
+    <t>543250080</t>
   </si>
   <si>
     <t>224564427</t>
@@ -61,6 +94,30 @@
     <t>545282162</t>
   </si>
   <si>
+    <t>24219149</t>
+  </si>
+  <si>
+    <t>כהן ערן</t>
+  </si>
+  <si>
+    <t>546644385</t>
+  </si>
+  <si>
+    <t>303054878</t>
+  </si>
+  <si>
+    <t>בן זאב אורי</t>
+  </si>
+  <si>
+    <t>526868697</t>
+  </si>
+  <si>
+    <t>7010070</t>
+  </si>
+  <si>
+    <t>רשם הערה בעת ההרשמה לתחרות</t>
+  </si>
+  <si>
     <t>7137</t>
   </si>
   <si>
@@ -79,7 +136,19 @@
     <t>לשנות לדן גרדי</t>
   </si>
   <si>
-    <t>רשם הערה בעת ההרשמה לתחרות</t>
+    <t>6744</t>
+  </si>
+  <si>
+    <t>צופה אלעד</t>
+  </si>
+  <si>
+    <t>טכניון כרמל</t>
+  </si>
+  <si>
+    <t>052-4044409</t>
+  </si>
+  <si>
+    <t>2071510</t>
   </si>
 </sst>
 </file>
@@ -411,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -490,20 +559,131 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="D5" t="s">
         <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>